<commit_message>
+updated: diagnosed cases list --> work-in-progress
</commit_message>
<xml_diff>
--- a/generateMonthlySummaryReport/Add-on Software Installer/assets/diagnosedCasesList.xlsx
+++ b/generateMonthlySummaryReport/Add-on Software Installer/assets/diagnosedCasesList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Usbong\STA LUCIA rehab\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\GitHub\mosc\generateMonthlySummaryReport\Add-on Software Installer\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>STL UE</t>
   </si>
@@ -38,18 +38,12 @@
     <t>Lateral Epicondylitis</t>
   </si>
   <si>
-    <t>Muscle Sprain/strain shoulder/elbow/wrist</t>
-  </si>
-  <si>
     <t>TFCC</t>
   </si>
   <si>
     <t>STL LE</t>
   </si>
   <si>
-    <t>Muscle Strain/Sprain Thigh/Leg/Ankle</t>
-  </si>
-  <si>
     <t>ACL injury</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>cervical Radiculopathy</t>
   </si>
   <si>
-    <t>Cervical spondylolysis/losis/listhesis</t>
-  </si>
-  <si>
     <t>Cervical spasm</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>lumbar disc bulge</t>
   </si>
   <si>
-    <t>Lumbar spondylosis/lolysis/listhesis</t>
-  </si>
-  <si>
     <t>Chronic LBP</t>
   </si>
   <si>
@@ -104,12 +92,6 @@
     <t>OA/RA/Gouty arthritis</t>
   </si>
   <si>
-    <t>hip/knee/ankle</t>
-  </si>
-  <si>
-    <t>UE/LE</t>
-  </si>
-  <si>
     <t>Scoliosis</t>
   </si>
   <si>
@@ -134,12 +116,6 @@
     <t>Lumbar Stenosis</t>
   </si>
   <si>
-    <t>Achilles Tendinitis/ Bursitis</t>
-  </si>
-  <si>
-    <t>Contusions/Bursitis</t>
-  </si>
-  <si>
     <t>CVA</t>
   </si>
   <si>
@@ -156,6 +132,117 @@
   </si>
   <si>
     <t>Lumbar disorder</t>
+  </si>
+  <si>
+    <t>Contusions</t>
+  </si>
+  <si>
+    <t>Bursitis</t>
+  </si>
+  <si>
+    <t>Muscle Sprain</t>
+  </si>
+  <si>
+    <t>Muscle strain shoulder</t>
+  </si>
+  <si>
+    <t>Muscle elbow</t>
+  </si>
+  <si>
+    <t>Muscle wrist</t>
+  </si>
+  <si>
+    <t>Muscle Strain</t>
+  </si>
+  <si>
+    <t>Muscle Sprain Thigh</t>
+  </si>
+  <si>
+    <t>Muscle Leg</t>
+  </si>
+  <si>
+    <t>Muscle Ankle</t>
+  </si>
+  <si>
+    <t>Achilles Tendinitis</t>
+  </si>
+  <si>
+    <t>Achilles Bursitis</t>
+  </si>
+  <si>
+    <t>Cervical spondylolysis</t>
+  </si>
+  <si>
+    <t>Cervical losis</t>
+  </si>
+  <si>
+    <t>Cervical listhesis</t>
+  </si>
+  <si>
+    <t>Lumbar spondylosis</t>
+  </si>
+  <si>
+    <t>Lumbar lolysis</t>
+  </si>
+  <si>
+    <t>Lumbar listhesis</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>Gouty arthritis</t>
+  </si>
+  <si>
+    <t>hip</t>
+  </si>
+  <si>
+    <t>knee</t>
+  </si>
+  <si>
+    <t>ankle</t>
+  </si>
+  <si>
+    <t>Fx/S/p ORIF</t>
+  </si>
+  <si>
+    <t>Fx/S/p Plating</t>
+  </si>
+  <si>
+    <t>Fx/S/p Screws</t>
+  </si>
+  <si>
+    <t>Fx/S/p Dislocation</t>
+  </si>
+  <si>
+    <t>UE</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>Trigger Finger</t>
+  </si>
+  <si>
+    <t>Stenosing tenosynovitis</t>
+  </si>
+  <si>
+    <t>Shoulder impingement</t>
+  </si>
+  <si>
+    <t>Shoulder rotator cuff tendinitis</t>
+  </si>
+  <si>
+    <t>Shoulder adhesive capsulitis</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>Cerebral Palsy</t>
   </si>
 </sst>
 </file>
@@ -505,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,10 +605,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,263 +656,455 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>